<commit_message>
add dodecane and a general example for mixtures
</commit_message>
<xml_diff>
--- a/fuelData/initData/decane_init.xlsx
+++ b/fuelData/initData/decane_init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abinswan/Documents/GroupContributionMethod/Init_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/dmontgo2_nrel_gov/Documents/Projects/SAF-VTO/GCM/MulticomponentEvaporation/GroupContributionMethod/fuelData/initData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52265D14-B2D0-6943-BF1E-EB22493461CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{52265D14-B2D0-6943-BF1E-EB22493461CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{713B033F-820D-3E47-8BDD-D494EF9948D8}"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="1280" windowWidth="23600" windowHeight="12040" tabRatio="141" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27200" yWindow="4480" windowWidth="23600" windowHeight="12040" tabRatio="141" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,7 +414,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -443,4 +443,10 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{95965d95-ecc0-4720-b759-1f33c42ed7da}" enabled="1" method="Standard" siteId="{a0f29d7e-28cd-4f54-8442-7885aee7c080}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>